<commit_message>
Some feature table enhancements
</commit_message>
<xml_diff>
--- a/xslt-collection/features.xlsx
+++ b/xslt-collection/features.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="106">
   <si>
     <t>00-musicxml</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>not supported</t>
-  </si>
-  <si>
-    <t>trivial</t>
   </si>
   <si>
     <t>non-trivial</t>
@@ -289,9 +286,6 @@
     <t>&lt;xsl:import&gt; or &lt;xsl:include&gt;</t>
   </si>
   <si>
-    <t>Named Templates</t>
-  </si>
-  <si>
     <t>Template Modes</t>
   </si>
   <si>
@@ -405,6 +399,18 @@
   </si>
   <si>
     <t>Attribute Value Templates</t>
+  </si>
+  <si>
+    <t>Named Templates (&lt;xsl:call-template&gt;) [*]</t>
+  </si>
+  <si>
+    <t>[*] &lt;xsl:apply-templates&gt; is implicitly used by all stylesheets in their built-in template rules, and therefore not listed here</t>
+  </si>
+  <si>
+    <t>trivial [**]</t>
+  </si>
+  <si>
+    <t>[**] A trivial descendant step is a descendant step ('//') as the first (leftmost) step in a pattern. A pattern with such a step is equivalent to the same pattern without that descendant step, because every element is a descendant of the root node.</t>
   </si>
 </sst>
 </file>
@@ -498,20 +504,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -531,12 +538,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -548,19 +549,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -918,17 +924,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="27" style="38" customWidth="1"/>
-    <col min="2" max="2" width="15" style="13" customWidth="1"/>
+    <col min="1" max="1" width="27" style="18" customWidth="1"/>
+    <col min="2" max="2" width="15" style="12" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
@@ -947,8 +953,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
@@ -999,10 +1005,10 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="36"/>
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1053,10 +1059,10 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="15"/>
+      <c r="A3" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="40"/>
       <c r="C3" t="s">
         <v>27</v>
       </c>
@@ -1107,10 +1113,10 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="34"/>
       <c r="C4" t="s">
         <v>35</v>
       </c>
@@ -1161,10 +1167,10 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="23"/>
+      <c r="A5" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="24"/>
       <c r="C5" t="s">
         <v>35</v>
       </c>
@@ -1215,10 +1221,10 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="19"/>
+      <c r="A6" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="34"/>
       <c r="C6" t="s">
         <v>35</v>
       </c>
@@ -1269,10 +1275,10 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="19"/>
+      <c r="A7" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="34"/>
       <c r="C7" t="s">
         <v>35</v>
       </c>
@@ -1323,10 +1329,10 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="33"/>
+      <c r="A8" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="20"/>
       <c r="C8" t="s">
         <v>35</v>
       </c>
@@ -1377,10 +1383,10 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="17"/>
+      <c r="A9" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="36"/>
       <c r="C9" t="s">
         <v>35</v>
       </c>
@@ -1431,10 +1437,10 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="6" t="s">
         <v>36</v>
       </c>
@@ -1485,10 +1491,10 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="21"/>
+      <c r="A11" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="22"/>
       <c r="C11" s="6" t="s">
         <v>36</v>
       </c>
@@ -1539,118 +1545,118 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>35</v>
+      </c>
+      <c r="R13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" t="s">
-        <v>35</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>35</v>
-      </c>
-      <c r="R12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P13" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>35</v>
-      </c>
-      <c r="R13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1701,442 +1707,442 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>35</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>35</v>
+      </c>
+      <c r="R16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M15" t="s">
-        <v>35</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O15" t="s">
-        <v>35</v>
-      </c>
-      <c r="P15" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>35</v>
-      </c>
-      <c r="R15" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K16" t="s">
-        <v>35</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O16" t="s">
-        <v>35</v>
-      </c>
-      <c r="P16" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>35</v>
-      </c>
-      <c r="R16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="20" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" t="s">
+        <v>35</v>
+      </c>
+      <c r="P18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>35</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" t="s">
+        <v>35</v>
+      </c>
+      <c r="P20" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>35</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" t="s">
+        <v>35</v>
+      </c>
+      <c r="P21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>35</v>
+      </c>
+      <c r="R21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" t="s">
+        <v>35</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P17" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" t="s">
-        <v>35</v>
-      </c>
-      <c r="M18" t="s">
-        <v>35</v>
-      </c>
-      <c r="N18" t="s">
-        <v>35</v>
-      </c>
-      <c r="O18" t="s">
-        <v>35</v>
-      </c>
-      <c r="P18" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>35</v>
-      </c>
-      <c r="R18" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" t="s">
-        <v>35</v>
-      </c>
-      <c r="L19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N19" t="s">
-        <v>35</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>35</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M20" t="s">
-        <v>35</v>
-      </c>
-      <c r="N20" t="s">
-        <v>35</v>
-      </c>
-      <c r="O20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>35</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K21" t="s">
-        <v>35</v>
-      </c>
-      <c r="L21" t="s">
-        <v>35</v>
-      </c>
-      <c r="M21" t="s">
-        <v>35</v>
-      </c>
-      <c r="N21" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21" t="s">
-        <v>35</v>
-      </c>
-      <c r="P21" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>35</v>
-      </c>
-      <c r="R21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="33"/>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J22" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L22" t="s">
-        <v>35</v>
-      </c>
-      <c r="M22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22" t="s">
-        <v>35</v>
-      </c>
-      <c r="P22" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="21"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="6" t="s">
         <v>36</v>
       </c>
@@ -2187,10 +2193,10 @@
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2241,10 +2247,10 @@
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="24"/>
       <c r="C25" t="s">
         <v>35</v>
       </c>
@@ -2295,10 +2301,10 @@
       </c>
     </row>
     <row r="26" spans="1:18" s="3" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A26" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="25"/>
+      <c r="A26" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="26"/>
       <c r="C26" s="4" t="s">
         <v>38</v>
       </c>
@@ -2349,10 +2355,10 @@
       </c>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="21"/>
+      <c r="A27" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="22"/>
       <c r="C27" s="6" t="s">
         <v>36</v>
       </c>
@@ -2403,8 +2409,8 @@
       </c>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="26" t="s">
-        <v>83</v>
+      <c r="A28" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>31</v>
@@ -2459,7 +2465,7 @@
       </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="26"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="11" t="s">
         <v>34</v>
       </c>
@@ -2513,7 +2519,7 @@
       </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="26"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="11" t="s">
         <v>33</v>
       </c>
@@ -2567,7 +2573,7 @@
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="26"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="11" t="s">
         <v>32</v>
       </c>
@@ -2621,172 +2627,172 @@
       </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" t="s">
+        <v>35</v>
+      </c>
+      <c r="M32" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32" t="s">
+        <v>35</v>
+      </c>
+      <c r="O32" t="s">
+        <v>35</v>
+      </c>
+      <c r="P32" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>35</v>
+      </c>
+      <c r="R32" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="38"/>
+      <c r="B33" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" t="s">
+        <v>35</v>
+      </c>
+      <c r="J33" t="s">
+        <v>35</v>
+      </c>
+      <c r="K33" t="s">
+        <v>35</v>
+      </c>
+      <c r="L33" t="s">
+        <v>35</v>
+      </c>
+      <c r="M33" t="s">
+        <v>35</v>
+      </c>
+      <c r="N33" t="s">
+        <v>35</v>
+      </c>
+      <c r="O33" t="s">
+        <v>35</v>
+      </c>
+      <c r="P33" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>35</v>
+      </c>
+      <c r="R33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="22"/>
+      <c r="C34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K34" t="s">
+        <v>35</v>
+      </c>
+      <c r="L34" t="s">
+        <v>35</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N34" t="s">
+        <v>35</v>
+      </c>
+      <c r="O34" t="s">
+        <v>35</v>
+      </c>
+      <c r="P34" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>35</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="37" t="s">
         <v>84</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" t="s">
-        <v>35</v>
-      </c>
-      <c r="G32" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" t="s">
-        <v>35</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K32" t="s">
-        <v>35</v>
-      </c>
-      <c r="L32" t="s">
-        <v>35</v>
-      </c>
-      <c r="M32" t="s">
-        <v>35</v>
-      </c>
-      <c r="N32" t="s">
-        <v>35</v>
-      </c>
-      <c r="O32" t="s">
-        <v>35</v>
-      </c>
-      <c r="P32" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>35</v>
-      </c>
-      <c r="R32" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18">
-      <c r="A33" s="27"/>
-      <c r="B33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H33" t="s">
-        <v>35</v>
-      </c>
-      <c r="I33" t="s">
-        <v>35</v>
-      </c>
-      <c r="J33" t="s">
-        <v>35</v>
-      </c>
-      <c r="K33" t="s">
-        <v>35</v>
-      </c>
-      <c r="L33" t="s">
-        <v>35</v>
-      </c>
-      <c r="M33" t="s">
-        <v>35</v>
-      </c>
-      <c r="N33" t="s">
-        <v>35</v>
-      </c>
-      <c r="O33" t="s">
-        <v>35</v>
-      </c>
-      <c r="P33" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>35</v>
-      </c>
-      <c r="R33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18">
-      <c r="A34" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K34" t="s">
-        <v>35</v>
-      </c>
-      <c r="L34" t="s">
-        <v>35</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N34" t="s">
-        <v>35</v>
-      </c>
-      <c r="O34" t="s">
-        <v>35</v>
-      </c>
-      <c r="P34" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>35</v>
-      </c>
-      <c r="R34" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18">
-      <c r="A35" s="26" t="s">
-        <v>86</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>31</v>
@@ -2841,7 +2847,7 @@
       </c>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="26"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="11" t="s">
         <v>34</v>
       </c>
@@ -2895,7 +2901,7 @@
       </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="26"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="11" t="s">
         <v>33</v>
       </c>
@@ -2949,7 +2955,7 @@
       </c>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="26"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="11" t="s">
         <v>32</v>
       </c>
@@ -3003,10 +3009,10 @@
       </c>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="21"/>
+      <c r="A39" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="22"/>
       <c r="C39" t="s">
         <v>35</v>
       </c>
@@ -3057,265 +3063,279 @@
       </c>
     </row>
     <row r="40" spans="1:18" s="3" customFormat="1" ht="140.25">
-      <c r="A40" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="25"/>
+      <c r="A40" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="26"/>
       <c r="C40" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D40" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="G40" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I40" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F40" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="J40" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K40" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M40" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="N40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O40" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="P40" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q40" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="R40" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H41" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" t="s">
+        <v>35</v>
+      </c>
+      <c r="L41" t="s">
+        <v>35</v>
+      </c>
+      <c r="M41" t="s">
+        <v>35</v>
+      </c>
+      <c r="N41" t="s">
+        <v>35</v>
+      </c>
+      <c r="O41" t="s">
+        <v>35</v>
+      </c>
+      <c r="P41" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>35</v>
+      </c>
+      <c r="R41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="22"/>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42" t="s">
+        <v>35</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L42" t="s">
+        <v>35</v>
+      </c>
+      <c r="M42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N42" t="s">
+        <v>35</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>35</v>
+      </c>
+      <c r="R42" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" s="3" customFormat="1" ht="92.25" customHeight="1">
+      <c r="A43" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="30"/>
+      <c r="D43" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="M40" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="N40" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="O40" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="P40" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q40" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="R40" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
-      <c r="A41" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41" s="21"/>
-      <c r="C41" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F41" t="s">
-        <v>35</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H41" t="s">
-        <v>35</v>
-      </c>
-      <c r="I41" t="s">
-        <v>35</v>
-      </c>
-      <c r="J41" t="s">
-        <v>35</v>
-      </c>
-      <c r="K41" t="s">
-        <v>35</v>
-      </c>
-      <c r="L41" t="s">
-        <v>35</v>
-      </c>
-      <c r="M41" t="s">
-        <v>35</v>
-      </c>
-      <c r="N41" t="s">
-        <v>35</v>
-      </c>
-      <c r="O41" t="s">
-        <v>35</v>
-      </c>
-      <c r="P41" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>35</v>
-      </c>
-      <c r="R41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18">
-      <c r="A42" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="21"/>
-      <c r="C42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" t="s">
-        <v>35</v>
-      </c>
-      <c r="F42" t="s">
-        <v>35</v>
-      </c>
-      <c r="G42" t="s">
-        <v>35</v>
-      </c>
-      <c r="H42" t="s">
-        <v>35</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L42" t="s">
-        <v>35</v>
-      </c>
-      <c r="M42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N42" t="s">
-        <v>35</v>
-      </c>
-      <c r="O42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>35</v>
-      </c>
-      <c r="R42" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" s="3" customFormat="1" ht="92.25" customHeight="1">
-      <c r="A43" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="31"/>
-      <c r="D43" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J43" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M43" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="M43" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="N43" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O43" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P43" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R43" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="O43" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="R43" s="8" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="44" spans="1:18" s="3" customFormat="1" ht="75" customHeight="1">
-      <c r="A44" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="29"/>
+      <c r="A44" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="28"/>
       <c r="D44" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>22</v>
       </c>
       <c r="O44" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P44" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q44" s="5" t="s">
         <v>22</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:18">
-      <c r="A45" s="34"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="36" t="s">
+      <c r="A45" s="14"/>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="37" t="s">
+    <row r="54" spans="1:1">
+      <c r="A54" s="17" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="37">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A43:B43"/>
@@ -3332,19 +3352,15 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>

</xml_diff>

<commit_message>
Various improvements, e.g. better feature analysis of Attribute Value Templates
</commit_message>
<xml_diff>
--- a/xslt-collection/features.xlsx
+++ b/xslt-collection/features.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="108">
   <si>
     <t>00-musicxml</t>
   </si>
@@ -259,9 +259,6 @@
 count</t>
   </si>
   <si>
-    <t>concat</t>
-  </si>
-  <si>
     <t>&lt;xsl:processing-instruction&gt;</t>
   </si>
   <si>
@@ -414,6 +411,13 @@
   </si>
   <si>
     <t>Custom Template priorities</t>
+  </si>
+  <si>
+    <t>translate</t>
+  </si>
+  <si>
+    <t>concat
+local-name</t>
   </si>
 </sst>
 </file>
@@ -515,40 +519,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -569,6 +549,30 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -929,7 +933,7 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -955,8 +959,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
+      <c r="A1" s="32"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1007,10 +1011,10 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="37"/>
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1061,10 +1065,10 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="27"/>
+      <c r="A3" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="39"/>
       <c r="C3" t="s">
         <v>27</v>
       </c>
@@ -1115,10 +1119,10 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="35"/>
       <c r="C4" t="s">
         <v>35</v>
       </c>
@@ -1169,10 +1173,10 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="35"/>
+      <c r="A5" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="23"/>
       <c r="C5" t="s">
         <v>35</v>
       </c>
@@ -1223,10 +1227,10 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="21"/>
+      <c r="A6" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="35"/>
       <c r="C6" t="s">
         <v>35</v>
       </c>
@@ -1277,10 +1281,10 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="21"/>
+      <c r="A7" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="35"/>
       <c r="C7" t="s">
         <v>35</v>
       </c>
@@ -1331,10 +1335,10 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="33"/>
+      <c r="A8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="19"/>
       <c r="C8" t="s">
         <v>35</v>
       </c>
@@ -1385,10 +1389,10 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="23"/>
+      <c r="A9" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="37"/>
       <c r="C9" t="s">
         <v>35</v>
       </c>
@@ -1439,10 +1443,10 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="6" t="s">
         <v>36</v>
       </c>
@@ -1493,10 +1497,10 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="25"/>
+      <c r="A11" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="21"/>
       <c r="C11" s="6" t="s">
         <v>36</v>
       </c>
@@ -1547,10 +1551,10 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="25"/>
+      <c r="A12" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="21"/>
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -1601,118 +1605,118 @@
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>35</v>
+      </c>
+      <c r="R13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P13" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>35</v>
-      </c>
-      <c r="R13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="33"/>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" t="s">
-        <v>35</v>
-      </c>
-      <c r="L14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" t="s">
-        <v>35</v>
-      </c>
-      <c r="N14" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" t="s">
-        <v>35</v>
-      </c>
-      <c r="P14" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>35</v>
-      </c>
-      <c r="R14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1763,442 +1767,442 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>35</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>35</v>
+      </c>
+      <c r="R17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M16" t="s">
-        <v>35</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O16" t="s">
-        <v>35</v>
-      </c>
-      <c r="P16" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>35</v>
-      </c>
-      <c r="R16" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="25"/>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O17" t="s">
-        <v>35</v>
-      </c>
-      <c r="P17" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>35</v>
-      </c>
-      <c r="R17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="24" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" t="s">
+        <v>35</v>
+      </c>
+      <c r="P19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P20" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>35</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" t="s">
+        <v>35</v>
+      </c>
+      <c r="P21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>35</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" t="s">
+        <v>35</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" t="s">
+        <v>35</v>
+      </c>
+      <c r="P23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>35</v>
+      </c>
+      <c r="R23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P18" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R18" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" t="s">
-        <v>35</v>
-      </c>
-      <c r="L19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M19" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" t="s">
-        <v>35</v>
-      </c>
-      <c r="O19" t="s">
-        <v>35</v>
-      </c>
-      <c r="P19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>35</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N20" t="s">
-        <v>35</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>35</v>
-      </c>
-      <c r="R20" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" t="s">
-        <v>35</v>
-      </c>
-      <c r="L21" t="s">
-        <v>35</v>
-      </c>
-      <c r="M21" t="s">
-        <v>35</v>
-      </c>
-      <c r="N21" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21" t="s">
-        <v>35</v>
-      </c>
-      <c r="P21" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>35</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="35"/>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L22" t="s">
-        <v>35</v>
-      </c>
-      <c r="M22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22" t="s">
-        <v>35</v>
-      </c>
-      <c r="P22" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="33"/>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L23" t="s">
-        <v>35</v>
-      </c>
-      <c r="M23" t="s">
-        <v>35</v>
-      </c>
-      <c r="N23" t="s">
-        <v>35</v>
-      </c>
-      <c r="O23" t="s">
-        <v>35</v>
-      </c>
-      <c r="P23" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>35</v>
-      </c>
-      <c r="R23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="25"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="6" t="s">
         <v>36</v>
       </c>
@@ -2249,10 +2253,10 @@
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="1" t="s">
         <v>36</v>
       </c>
@@ -2303,10 +2307,10 @@
       </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="23"/>
       <c r="C26" t="s">
         <v>35</v>
       </c>
@@ -2357,10 +2361,10 @@
       </c>
     </row>
     <row r="27" spans="1:18" s="3" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A27" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="37"/>
+      <c r="A27" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="25"/>
       <c r="C27" s="4" t="s">
         <v>38</v>
       </c>
@@ -2411,62 +2415,62 @@
       </c>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" t="s">
+        <v>35</v>
+      </c>
+      <c r="M28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N28" t="s">
+        <v>35</v>
+      </c>
+      <c r="O28" t="s">
+        <v>35</v>
+      </c>
+      <c r="P28" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>35</v>
+      </c>
+      <c r="R28" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="26" t="s">
         <v>80</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" t="s">
-        <v>35</v>
-      </c>
-      <c r="L28" t="s">
-        <v>35</v>
-      </c>
-      <c r="M28" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" t="s">
-        <v>35</v>
-      </c>
-      <c r="O28" t="s">
-        <v>35</v>
-      </c>
-      <c r="P28" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>35</v>
-      </c>
-      <c r="R28" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="38" t="s">
-        <v>81</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>31</v>
@@ -2521,7 +2525,7 @@
       </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="38"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="11" t="s">
         <v>34</v>
       </c>
@@ -2575,7 +2579,7 @@
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="38"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="11" t="s">
         <v>33</v>
       </c>
@@ -2629,7 +2633,7 @@
       </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="38"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="11" t="s">
         <v>32</v>
       </c>
@@ -2683,11 +2687,11 @@
       </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="39" t="s">
-        <v>82</v>
+      <c r="A33" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
@@ -2739,7 +2743,7 @@
       </c>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="39"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="10" t="s">
         <v>46</v>
       </c>
@@ -2793,62 +2797,62 @@
       </c>
     </row>
     <row r="35" spans="1:18">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K35" t="s">
+        <v>35</v>
+      </c>
+      <c r="L35" t="s">
+        <v>35</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N35" t="s">
+        <v>35</v>
+      </c>
+      <c r="O35" t="s">
+        <v>35</v>
+      </c>
+      <c r="P35" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>35</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="26" t="s">
         <v>83</v>
-      </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" t="s">
-        <v>35</v>
-      </c>
-      <c r="F35" t="s">
-        <v>35</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K35" t="s">
-        <v>35</v>
-      </c>
-      <c r="L35" t="s">
-        <v>35</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N35" t="s">
-        <v>35</v>
-      </c>
-      <c r="O35" t="s">
-        <v>35</v>
-      </c>
-      <c r="P35" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>35</v>
-      </c>
-      <c r="R35" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18">
-      <c r="A36" s="38" t="s">
-        <v>84</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>31</v>
@@ -2903,7 +2907,7 @@
       </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="38"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="11" t="s">
         <v>34</v>
       </c>
@@ -2957,7 +2961,7 @@
       </c>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="38"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="11" t="s">
         <v>33</v>
       </c>
@@ -3011,7 +3015,7 @@
       </c>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="38"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="11" t="s">
         <v>32</v>
       </c>
@@ -3065,84 +3069,84 @@
       </c>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="21"/>
+      <c r="C40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J40" t="s">
+        <v>35</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M40" t="s">
+        <v>35</v>
+      </c>
+      <c r="N40" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" t="s">
+        <v>35</v>
+      </c>
+      <c r="P40" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R40" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" s="3" customFormat="1" ht="140.25">
+      <c r="A41" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" t="s">
-        <v>35</v>
-      </c>
-      <c r="G40" t="s">
-        <v>35</v>
-      </c>
-      <c r="H40" t="s">
-        <v>35</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J40" t="s">
-        <v>35</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L40" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M40" t="s">
-        <v>35</v>
-      </c>
-      <c r="N40" t="s">
-        <v>35</v>
-      </c>
-      <c r="O40" t="s">
-        <v>35</v>
-      </c>
-      <c r="P40" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R40" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" s="3" customFormat="1" ht="140.25">
-      <c r="A41" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" s="37"/>
+      <c r="B41" s="25"/>
       <c r="C41" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D41" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="G41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>47</v>
@@ -3154,83 +3158,83 @@
         <v>47</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N41" s="8" t="s">
         <v>47</v>
       </c>
       <c r="O41" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="P41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q41" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="P41" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q41" s="8" t="s">
-        <v>100</v>
-      </c>
       <c r="R41" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F42" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42" t="s">
+        <v>35</v>
+      </c>
+      <c r="I42" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" t="s">
+        <v>35</v>
+      </c>
+      <c r="L42" t="s">
+        <v>35</v>
+      </c>
+      <c r="M42" t="s">
+        <v>35</v>
+      </c>
+      <c r="N42" t="s">
+        <v>35</v>
+      </c>
+      <c r="O42" t="s">
+        <v>35</v>
+      </c>
+      <c r="P42" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>35</v>
+      </c>
+      <c r="R42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F42" t="s">
-        <v>35</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H42" t="s">
-        <v>35</v>
-      </c>
-      <c r="I42" t="s">
-        <v>35</v>
-      </c>
-      <c r="J42" t="s">
-        <v>35</v>
-      </c>
-      <c r="K42" t="s">
-        <v>35</v>
-      </c>
-      <c r="L42" t="s">
-        <v>35</v>
-      </c>
-      <c r="M42" t="s">
-        <v>35</v>
-      </c>
-      <c r="N42" t="s">
-        <v>35</v>
-      </c>
-      <c r="O42" t="s">
-        <v>35</v>
-      </c>
-      <c r="P42" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>35</v>
-      </c>
-      <c r="R42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18">
-      <c r="A43" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="21"/>
       <c r="C43" t="s">
         <v>35</v>
       </c>
@@ -3282,7 +3286,7 @@
     </row>
     <row r="44" spans="1:18" s="3" customFormat="1" ht="92.25" customHeight="1">
       <c r="A44" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="31"/>
       <c r="D44" s="8" t="s">
@@ -3313,12 +3317,12 @@
         <v>61</v>
       </c>
       <c r="R44" s="8" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="3" customFormat="1" ht="75" customHeight="1">
       <c r="A45" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B45" s="29"/>
       <c r="D45" s="4" t="s">
@@ -3327,6 +3331,9 @@
       <c r="G45" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="H45" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="I45" s="4" t="s">
         <v>52</v>
       </c>
@@ -3354,17 +3361,17 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:1">
@@ -3380,19 +3387,15 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="38">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A44:B44"/>
@@ -3409,15 +3412,19 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
last() function is supported
</commit_message>
<xml_diff>
--- a/xslt-collection/features.xlsx
+++ b/xslt-collection/features.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="107">
   <si>
     <t>00-musicxml</t>
   </si>
@@ -206,24 +206,6 @@
 number</t>
   </si>
   <si>
-    <t>document
-normalize-space
-namespace-uri
-last</t>
-  </si>
-  <si>
-    <t>count
-position
-local-name</t>
-  </si>
-  <si>
-    <t>last</t>
-  </si>
-  <si>
-    <t>position
-string</t>
-  </si>
-  <si>
     <t>string
 not
 concat</t>
@@ -418,6 +400,22 @@
   <si>
     <t>concat
 local-name</t>
+  </si>
+  <si>
+    <t>position
+string
+last</t>
+  </si>
+  <si>
+    <t>count
+position
+local-name
+last</t>
+  </si>
+  <si>
+    <t>document
+normalize-space
+namespace-uri</t>
   </si>
 </sst>
 </file>
@@ -437,7 +435,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,6 +457,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -519,16 +523,40 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,30 +577,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -959,8 +966,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1011,10 +1018,10 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="23"/>
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1065,10 +1072,10 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="39"/>
+      <c r="A3" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="27"/>
       <c r="C3" t="s">
         <v>27</v>
       </c>
@@ -1119,10 +1126,10 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="21"/>
       <c r="C4" t="s">
         <v>35</v>
       </c>
@@ -1173,226 +1180,226 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="35"/>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="35"/>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" t="s">
-        <v>35</v>
-      </c>
-      <c r="P8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="23"/>
       <c r="C9" t="s">
         <v>35</v>
       </c>
@@ -1443,10 +1450,10 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="6" t="s">
         <v>36</v>
       </c>
@@ -1497,10 +1504,10 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="21"/>
+      <c r="A11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="25"/>
       <c r="C11" s="6" t="s">
         <v>36</v>
       </c>
@@ -1551,118 +1558,118 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>35</v>
+      </c>
+      <c r="R13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" t="s">
-        <v>35</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>35</v>
-      </c>
-      <c r="R12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P13" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>35</v>
-      </c>
-      <c r="R13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="33"/>
       <c r="C14" t="s">
         <v>35</v>
       </c>
@@ -1713,10 +1720,10 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="23"/>
+      <c r="A15" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="35"/>
       <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1767,10 +1774,10 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="21"/>
+      <c r="A16" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="25"/>
       <c r="C16" t="s">
         <v>35</v>
       </c>
@@ -1821,10 +1828,10 @@
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="21"/>
+      <c r="A17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="25"/>
       <c r="C17" t="s">
         <v>35</v>
       </c>
@@ -1875,10 +1882,10 @@
       </c>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="21"/>
+      <c r="A18" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="25"/>
       <c r="C18" t="s">
         <v>35</v>
       </c>
@@ -1929,280 +1936,280 @@
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" t="s">
+        <v>35</v>
+      </c>
+      <c r="P19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P20" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>35</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" t="s">
+        <v>35</v>
+      </c>
+      <c r="P21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>35</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="35"/>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" t="s">
+        <v>35</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="33"/>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" t="s">
+        <v>35</v>
+      </c>
+      <c r="P23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>35</v>
+      </c>
+      <c r="R23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" t="s">
-        <v>35</v>
-      </c>
-      <c r="L19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M19" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" t="s">
-        <v>35</v>
-      </c>
-      <c r="O19" t="s">
-        <v>35</v>
-      </c>
-      <c r="P19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>35</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N20" t="s">
-        <v>35</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>35</v>
-      </c>
-      <c r="R20" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" t="s">
-        <v>35</v>
-      </c>
-      <c r="L21" t="s">
-        <v>35</v>
-      </c>
-      <c r="M21" t="s">
-        <v>35</v>
-      </c>
-      <c r="N21" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21" t="s">
-        <v>35</v>
-      </c>
-      <c r="P21" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>35</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="23"/>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L22" t="s">
-        <v>35</v>
-      </c>
-      <c r="M22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22" t="s">
-        <v>35</v>
-      </c>
-      <c r="P22" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L23" t="s">
-        <v>35</v>
-      </c>
-      <c r="M23" t="s">
-        <v>35</v>
-      </c>
-      <c r="N23" t="s">
-        <v>35</v>
-      </c>
-      <c r="O23" t="s">
-        <v>35</v>
-      </c>
-      <c r="P23" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>35</v>
-      </c>
-      <c r="R23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="21"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="6" t="s">
         <v>36</v>
       </c>
@@ -2253,10 +2260,10 @@
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="1" t="s">
         <v>36</v>
       </c>
@@ -2307,10 +2314,10 @@
       </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="35"/>
       <c r="C26" t="s">
         <v>35</v>
       </c>
@@ -2361,10 +2368,10 @@
       </c>
     </row>
     <row r="27" spans="1:18" s="3" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A27" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="25"/>
+      <c r="A27" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="37"/>
       <c r="C27" s="4" t="s">
         <v>38</v>
       </c>
@@ -2415,10 +2422,10 @@
       </c>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="21"/>
+      <c r="A28" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="25"/>
       <c r="C28" s="6" t="s">
         <v>36</v>
       </c>
@@ -2469,8 +2476,8 @@
       </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="26" t="s">
-        <v>80</v>
+      <c r="A29" s="38" t="s">
+        <v>76</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>31</v>
@@ -2525,7 +2532,7 @@
       </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="26"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="11" t="s">
         <v>34</v>
       </c>
@@ -2579,7 +2586,7 @@
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="26"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="11" t="s">
         <v>33</v>
       </c>
@@ -2633,7 +2640,7 @@
       </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="26"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="11" t="s">
         <v>32</v>
       </c>
@@ -2687,11 +2694,11 @@
       </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="27" t="s">
-        <v>81</v>
+      <c r="A33" s="39" t="s">
+        <v>77</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
@@ -2743,7 +2750,7 @@
       </c>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="27"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="10" t="s">
         <v>46</v>
       </c>
@@ -2797,10 +2804,10 @@
       </c>
     </row>
     <row r="35" spans="1:18">
-      <c r="A35" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="21"/>
+      <c r="A35" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="25"/>
       <c r="C35" s="6" t="s">
         <v>36</v>
       </c>
@@ -2851,8 +2858,8 @@
       </c>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="26" t="s">
-        <v>83</v>
+      <c r="A36" s="38" t="s">
+        <v>79</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>31</v>
@@ -2907,7 +2914,7 @@
       </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="26"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="11" t="s">
         <v>34</v>
       </c>
@@ -2961,7 +2968,7 @@
       </c>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="26"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="11" t="s">
         <v>33</v>
       </c>
@@ -3015,7 +3022,7 @@
       </c>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="26"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="11" t="s">
         <v>32</v>
       </c>
@@ -3069,10 +3076,10 @@
       </c>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" s="21"/>
+      <c r="A40" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="25"/>
       <c r="C40" t="s">
         <v>35</v>
       </c>
@@ -3123,30 +3130,30 @@
       </c>
     </row>
     <row r="41" spans="1:18" s="3" customFormat="1" ht="140.25">
-      <c r="A41" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="25"/>
+      <c r="A41" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="37"/>
       <c r="C41" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>47</v>
@@ -3158,29 +3165,29 @@
         <v>47</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="N41" s="8" t="s">
         <v>47</v>
       </c>
       <c r="O41" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P41" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q41" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="Q41" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="R41" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="21"/>
+      <c r="A42" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="25"/>
       <c r="C42" t="s">
         <v>35</v>
       </c>
@@ -3231,10 +3238,10 @@
       </c>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="21"/>
+      <c r="A43" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="25"/>
       <c r="C43" t="s">
         <v>35</v>
       </c>
@@ -3286,7 +3293,7 @@
     </row>
     <row r="44" spans="1:18" s="3" customFormat="1" ht="92.25" customHeight="1">
       <c r="A44" s="30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B44" s="31"/>
       <c r="D44" s="8" t="s">
@@ -3299,30 +3306,30 @@
         <v>51</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="J44" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M44" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N44" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O44" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="M44" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N44" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="O44" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="P44" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R44" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="3" customFormat="1" ht="75" customHeight="1">
       <c r="A45" s="28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B45" s="29"/>
       <c r="D45" s="4" t="s">
@@ -3332,25 +3339,23 @@
         <v>22</v>
       </c>
       <c r="H45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I45" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="J45" s="40"/>
       <c r="M45" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>22</v>
       </c>
       <c r="O45" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="P45" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q45" s="5" t="s">
         <v>22</v>
@@ -3361,17 +3366,17 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:1">
@@ -3387,15 +3392,18 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="38">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A44:B44"/>
@@ -3412,19 +3420,16 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Update thesis and feature table to reflect latest additions
</commit_message>
<xml_diff>
--- a/xslt-collection/features.xlsx
+++ b/xslt-collection/features.xlsx
@@ -512,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -556,41 +556,23 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -605,11 +587,31 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -996,8 +998,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="8" customFormat="1">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24"/>
+      <c r="A1" s="37"/>
+      <c r="B1" s="38"/>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1048,10 +1050,10 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="42"/>
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1102,10 +1104,10 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="44"/>
       <c r="C3" t="s">
         <v>26</v>
       </c>
@@ -1156,10 +1158,10 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="40"/>
       <c r="C4" t="s">
         <v>34</v>
       </c>
@@ -1210,10 +1212,10 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="28"/>
       <c r="C5" t="s">
         <v>34</v>
       </c>
@@ -1264,14 +1266,14 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="46"/>
       <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E6" t="s">
@@ -1280,7 +1282,7 @@
       <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H6" t="s">
@@ -1295,10 +1297,10 @@
       <c r="K6" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="L6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N6" t="s">
@@ -1307,7 +1309,7 @@
       <c r="O6" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q6" t="s">
@@ -1318,29 +1320,29 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="46"/>
       <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="5" t="s">
         <v>35</v>
       </c>
       <c r="J7" t="s">
@@ -1372,10 +1374,10 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="40"/>
+      <c r="B8" s="30"/>
       <c r="C8" t="s">
         <v>34</v>
       </c>
@@ -1480,10 +1482,10 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1534,10 +1536,10 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="30"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="5" t="s">
         <v>35</v>
       </c>
@@ -1588,10 +1590,10 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="30"/>
+      <c r="B12" s="24"/>
       <c r="C12" t="s">
         <v>34</v>
       </c>
@@ -1642,10 +1644,10 @@
       </c>
     </row>
     <row r="13" spans="1:18" s="2" customFormat="1">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="34"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="2" t="s">
         <v>111</v>
       </c>
@@ -1696,10 +1698,10 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="24"/>
       <c r="C14" t="s">
         <v>34</v>
       </c>
@@ -1750,10 +1752,10 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="40"/>
+      <c r="B15" s="30"/>
       <c r="C15" t="s">
         <v>34</v>
       </c>
@@ -1804,17 +1806,17 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F16" t="s">
@@ -1826,7 +1828,7 @@
       <c r="H16" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="J16" t="s">
@@ -1835,19 +1837,19 @@
       <c r="K16" t="s">
         <v>34</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="1" t="s">
+      <c r="L16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N16" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P16" s="1" t="s">
+      <c r="O16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q16" t="s">
@@ -1858,10 +1860,10 @@
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="30"/>
+      <c r="B17" s="24"/>
       <c r="C17" t="s">
         <v>34</v>
       </c>
@@ -1912,10 +1914,10 @@
       </c>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="30"/>
+      <c r="B18" s="24"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -1966,10 +1968,10 @@
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="24"/>
       <c r="C19" t="s">
         <v>34</v>
       </c>
@@ -2020,10 +2022,10 @@
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="30"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
@@ -2074,10 +2076,10 @@
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="30"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="5" t="s">
         <v>35</v>
       </c>
@@ -2128,10 +2130,10 @@
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="30"/>
+      <c r="B22" s="24"/>
       <c r="C22" t="s">
         <v>34</v>
       </c>
@@ -2182,10 +2184,10 @@
       </c>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="34"/>
+      <c r="B23" s="28"/>
       <c r="C23" t="s">
         <v>34</v>
       </c>
@@ -2236,10 +2238,10 @@
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="40"/>
+      <c r="B24" s="30"/>
       <c r="C24" t="s">
         <v>34</v>
       </c>
@@ -2290,10 +2292,10 @@
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="30"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="5" t="s">
         <v>35</v>
       </c>
@@ -2344,10 +2346,10 @@
       </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="30"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="5" t="s">
         <v>35</v>
       </c>
@@ -2398,10 +2400,10 @@
       </c>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="34"/>
+      <c r="B27" s="28"/>
       <c r="C27" t="s">
         <v>34</v>
       </c>
@@ -2452,10 +2454,10 @@
       </c>
     </row>
     <row r="28" spans="1:18" s="3" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="42"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="7" t="s">
         <v>37</v>
       </c>
@@ -2506,10 +2508,10 @@
       </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="30"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="5" t="s">
         <v>35</v>
       </c>
@@ -2560,7 +2562,7 @@
       </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="25" t="s">
         <v>75</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -2616,7 +2618,7 @@
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="43"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="10" t="s">
         <v>33</v>
       </c>
@@ -2670,7 +2672,7 @@
       </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="43"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="10" t="s">
         <v>32</v>
       </c>
@@ -2724,7 +2726,7 @@
       </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="43"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="10" t="s">
         <v>31</v>
       </c>
@@ -2778,7 +2780,7 @@
       </c>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="26" t="s">
         <v>76</v>
       </c>
       <c r="B34" s="12" t="s">
@@ -2834,7 +2836,7 @@
       </c>
     </row>
     <row r="35" spans="1:18">
-      <c r="A35" s="44"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="9" t="s">
         <v>45</v>
       </c>
@@ -2888,10 +2890,10 @@
       </c>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="30"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="5" t="s">
         <v>35</v>
       </c>
@@ -2942,7 +2944,7 @@
       </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="25" t="s">
         <v>78</v>
       </c>
       <c r="B37" s="10" t="s">
@@ -2998,7 +3000,7 @@
       </c>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="43"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="10" t="s">
         <v>33</v>
       </c>
@@ -3052,7 +3054,7 @@
       </c>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="43"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="10" t="s">
         <v>32</v>
       </c>
@@ -3106,7 +3108,7 @@
       </c>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="43"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="10" t="s">
         <v>31</v>
       </c>
@@ -3160,10 +3162,10 @@
       </c>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="30"/>
+      <c r="B41" s="24"/>
       <c r="C41" t="s">
         <v>34</v>
       </c>
@@ -3214,10 +3216,10 @@
       </c>
     </row>
     <row r="42" spans="1:18" s="3" customFormat="1" ht="140.25">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="42"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="7" t="s">
         <v>46</v>
       </c>
@@ -3268,10 +3270,10 @@
       </c>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="24"/>
       <c r="C43" t="s">
         <v>34</v>
       </c>
@@ -3322,10 +3324,10 @@
       </c>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="30"/>
+      <c r="B44" s="24"/>
       <c r="C44" t="s">
         <v>34</v>
       </c>
@@ -3376,10 +3378,10 @@
       </c>
     </row>
     <row r="45" spans="1:18" s="3" customFormat="1" ht="92.25" customHeight="1">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="38"/>
+      <c r="B45" s="36"/>
       <c r="D45" s="7" t="s">
         <v>47</v>
       </c>
@@ -3415,10 +3417,10 @@
       </c>
     </row>
     <row r="46" spans="1:18" s="3" customFormat="1" ht="75" customHeight="1">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="B46" s="36"/>
+      <c r="B46" s="34"/>
       <c r="D46" s="4" t="s">
         <v>49</v>
       </c>
@@ -3484,19 +3486,16 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="39">
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A45:B45"/>
@@ -3513,16 +3512,19 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed feature row "Recursive templates"
</commit_message>
<xml_diff>
--- a/xslt-collection/features.xlsx
+++ b/xslt-collection/features.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="110">
   <si>
     <t>00-musicxml</t>
   </si>
@@ -428,12 +428,6 @@
   </si>
   <si>
     <t>stubbed out</t>
-  </si>
-  <si>
-    <t>Recursive Template Evaluation</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -512,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -547,7 +541,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -555,24 +548,43 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -587,31 +599,11 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -969,7 +961,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -998,8 +990,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="8" customFormat="1">
-      <c r="A1" s="37"/>
-      <c r="B1" s="38"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1050,10 +1042,10 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="30"/>
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1104,10 +1096,10 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="32"/>
       <c r="C3" t="s">
         <v>26</v>
       </c>
@@ -1158,10 +1150,10 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="34"/>
       <c r="C4" t="s">
         <v>34</v>
       </c>
@@ -1212,10 +1204,10 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="26"/>
       <c r="C5" t="s">
         <v>34</v>
       </c>
@@ -1266,10 +1258,10 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="46"/>
+      <c r="B6" s="24"/>
       <c r="C6" t="s">
         <v>34</v>
       </c>
@@ -1320,10 +1312,10 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="46"/>
+      <c r="B7" s="24"/>
       <c r="C7" t="s">
         <v>34</v>
       </c>
@@ -1374,10 +1366,10 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="40"/>
       <c r="C8" t="s">
         <v>34</v>
       </c>
@@ -1428,10 +1420,10 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="26"/>
       <c r="C9" t="s">
         <v>34</v>
       </c>
@@ -1482,10 +1474,10 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="24"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1536,10 +1528,10 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="5" t="s">
         <v>35</v>
       </c>
@@ -1590,10 +1582,10 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="24"/>
+      <c r="B12" s="28"/>
       <c r="C12" t="s">
         <v>34</v>
       </c>
@@ -1643,76 +1635,76 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="2" customFormat="1">
+    <row r="13" spans="1:18">
       <c r="A13" s="27" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="B13" s="28"/>
-      <c r="C13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="L13" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>111</v>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="24"/>
+      <c r="A14" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="40"/>
       <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>35</v>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
       </c>
       <c r="G14" t="s">
         <v>34</v>
@@ -1720,8 +1712,8 @@
       <c r="H14" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>35</v>
+      <c r="I14" t="s">
+        <v>34</v>
       </c>
       <c r="J14" t="s">
         <v>34</v>
@@ -1729,8 +1721,8 @@
       <c r="K14" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>35</v>
+      <c r="L14" t="s">
+        <v>34</v>
       </c>
       <c r="M14" t="s">
         <v>34</v>
@@ -1738,8 +1730,8 @@
       <c r="N14" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="5" t="s">
-        <v>35</v>
+      <c r="O14" t="s">
+        <v>34</v>
       </c>
       <c r="P14" t="s">
         <v>34</v>
@@ -1752,18 +1744,18 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="30"/>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
+      <c r="A15" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="F15" t="s">
         <v>34</v>
@@ -1774,8 +1766,8 @@
       <c r="H15" t="s">
         <v>34</v>
       </c>
-      <c r="I15" t="s">
-        <v>34</v>
+      <c r="I15" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="J15" t="s">
         <v>34</v>
@@ -1783,20 +1775,20 @@
       <c r="K15" t="s">
         <v>34</v>
       </c>
-      <c r="L15" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" t="s">
-        <v>34</v>
+      <c r="L15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="N15" t="s">
         <v>34</v>
       </c>
-      <c r="O15" t="s">
-        <v>34</v>
-      </c>
-      <c r="P15" t="s">
-        <v>34</v>
+      <c r="O15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="Q15" t="s">
         <v>34</v>
@@ -1806,12 +1798,12 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="5" t="s">
-        <v>35</v>
+      <c r="A16" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" t="s">
+        <v>34</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>35</v>
@@ -1819,11 +1811,11 @@
       <c r="E16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" t="s">
-        <v>34</v>
+      <c r="F16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -1831,53 +1823,53 @@
       <c r="I16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" t="s">
-        <v>34</v>
+      <c r="J16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N16" t="s">
-        <v>34</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>35</v>
+      <c r="M16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16" t="s">
+        <v>34</v>
       </c>
       <c r="Q16" t="s">
         <v>34</v>
       </c>
-      <c r="R16" t="s">
-        <v>34</v>
+      <c r="R16" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="24"/>
+      <c r="A17" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="28"/>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>35</v>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
       </c>
       <c r="H17" t="s">
         <v>34</v>
@@ -1888,14 +1880,14 @@
       <c r="J17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>35</v>
+      <c r="K17" t="s">
+        <v>34</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M17" t="s">
-        <v>34</v>
+      <c r="M17" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="N17" s="5" t="s">
         <v>35</v>
@@ -1909,29 +1901,29 @@
       <c r="Q17" t="s">
         <v>34</v>
       </c>
-      <c r="R17" s="5" t="s">
-        <v>35</v>
+      <c r="R17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="24"/>
+      <c r="A18" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="28"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" t="s">
-        <v>34</v>
+      <c r="E18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
@@ -1942,8 +1934,8 @@
       <c r="J18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K18" t="s">
-        <v>34</v>
+      <c r="K18" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>35</v>
@@ -1951,81 +1943,81 @@
       <c r="M18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O18" t="s">
-        <v>34</v>
+      <c r="N18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="P18" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" t="s">
-        <v>34</v>
-      </c>
-      <c r="R18" t="s">
-        <v>34</v>
+      <c r="Q18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" t="s">
-        <v>34</v>
+      <c r="A19" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" t="s">
-        <v>34</v>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>35</v>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19" t="s">
+        <v>34</v>
       </c>
       <c r="P19" t="s">
         <v>34</v>
       </c>
-      <c r="Q19" s="5" t="s">
-        <v>35</v>
+      <c r="Q19" t="s">
+        <v>34</v>
       </c>
       <c r="R19" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="24"/>
+      <c r="A20" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="28"/>
       <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
@@ -2038,11 +2030,11 @@
       <c r="F20" t="s">
         <v>34</v>
       </c>
-      <c r="G20" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>35</v>
+      <c r="G20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
+        <v>34</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>35</v>
@@ -2056,14 +2048,14 @@
       <c r="L20" t="s">
         <v>34</v>
       </c>
-      <c r="M20" t="s">
-        <v>34</v>
+      <c r="M20" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="N20" t="s">
         <v>34</v>
       </c>
-      <c r="O20" t="s">
-        <v>34</v>
+      <c r="O20" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="P20" t="s">
         <v>34</v>
@@ -2076,27 +2068,27 @@
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="5" t="s">
-        <v>35</v>
+      <c r="A21" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" t="s">
+        <v>34</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
+      <c r="E21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H21" t="s">
-        <v>34</v>
+      <c r="H21" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>35</v>
@@ -2107,11 +2099,11 @@
       <c r="K21" t="s">
         <v>34</v>
       </c>
-      <c r="L21" t="s">
-        <v>34</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>35</v>
+      <c r="L21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" t="s">
+        <v>34</v>
       </c>
       <c r="N21" t="s">
         <v>34</v>
@@ -2122,47 +2114,47 @@
       <c r="P21" t="s">
         <v>34</v>
       </c>
-      <c r="Q21" t="s">
-        <v>34</v>
+      <c r="Q21" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="R21" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="24"/>
+      <c r="A22" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="26"/>
       <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J22" t="s">
-        <v>34</v>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="K22" t="s">
         <v>34</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>35</v>
+      <c r="L22" t="s">
+        <v>34</v>
       </c>
       <c r="M22" t="s">
         <v>34</v>
@@ -2170,32 +2162,32 @@
       <c r="N22" t="s">
         <v>34</v>
       </c>
-      <c r="O22" s="5" t="s">
-        <v>35</v>
+      <c r="O22" t="s">
+        <v>34</v>
       </c>
       <c r="P22" t="s">
         <v>34</v>
       </c>
-      <c r="Q22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>35</v>
+      <c r="Q22" t="s">
+        <v>34</v>
+      </c>
+      <c r="R22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="28"/>
+      <c r="A23" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="40"/>
       <c r="C23" t="s">
         <v>34</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>35</v>
+      <c r="E23" t="s">
+        <v>34</v>
       </c>
       <c r="F23" t="s">
         <v>34</v>
@@ -2209,8 +2201,8 @@
       <c r="I23" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>35</v>
+      <c r="J23" t="s">
+        <v>34</v>
       </c>
       <c r="K23" t="s">
         <v>34</v>
@@ -2238,64 +2230,64 @@
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="30"/>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
+      <c r="A24" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
       </c>
-      <c r="G24" t="s">
-        <v>34</v>
+      <c r="G24" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="H24" t="s">
         <v>34</v>
       </c>
-      <c r="I24" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" t="s">
-        <v>34</v>
-      </c>
-      <c r="K24" t="s">
-        <v>34</v>
+      <c r="I24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="L24" t="s">
         <v>34</v>
       </c>
-      <c r="M24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O24" t="s">
-        <v>34</v>
-      </c>
-      <c r="P24" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>34</v>
+      <c r="M24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="R24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="24"/>
+      <c r="A25" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="28"/>
       <c r="C25" s="5" t="s">
         <v>35</v>
       </c>
@@ -2308,8 +2300,8 @@
       <c r="F25" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>35</v>
+      <c r="G25" t="s">
+        <v>34</v>
       </c>
       <c r="H25" t="s">
         <v>34</v>
@@ -2332,32 +2324,32 @@
       <c r="N25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>35</v>
+      <c r="O25" t="s">
+        <v>34</v>
+      </c>
+      <c r="P25" t="s">
+        <v>34</v>
       </c>
       <c r="Q25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="R25" t="s">
-        <v>34</v>
+      <c r="R25" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>35</v>
+      <c r="A26" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
       </c>
       <c r="F26" t="s">
         <v>34</v>
@@ -2368,23 +2360,23 @@
       <c r="H26" t="s">
         <v>34</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>35</v>
+      <c r="I26" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" t="s">
+        <v>34</v>
       </c>
       <c r="L26" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>35</v>
+      <c r="M26" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" t="s">
+        <v>34</v>
       </c>
       <c r="O26" t="s">
         <v>34</v>
@@ -2392,131 +2384,133 @@
       <c r="P26" t="s">
         <v>34</v>
       </c>
-      <c r="Q26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R26" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18">
-      <c r="A27" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K27" t="s">
-        <v>34</v>
-      </c>
-      <c r="L27" t="s">
-        <v>34</v>
-      </c>
-      <c r="M27" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" t="s">
-        <v>34</v>
-      </c>
-      <c r="O27" t="s">
-        <v>34</v>
-      </c>
-      <c r="P27" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>34</v>
-      </c>
-      <c r="R27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="3" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A28" s="31" t="s">
+      <c r="Q26" t="s">
+        <v>34</v>
+      </c>
+      <c r="R26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="3" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A27" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="7" t="s">
+      <c r="B27" s="42"/>
+      <c r="C27" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="J27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K27" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L28" s="7" t="s">
+      <c r="L27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M28" s="6" t="s">
+      <c r="M27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N28" s="6" t="s">
+      <c r="N27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O28" s="6" t="s">
+      <c r="O27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P28" s="7" t="s">
+      <c r="P27" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Q28" s="6" t="s">
+      <c r="Q27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="R28" s="7" t="s">
+      <c r="R27" s="7" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" t="s">
+        <v>34</v>
+      </c>
+      <c r="O28" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>34</v>
+      </c>
+      <c r="R28" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>35</v>
+      <c r="A29" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>34</v>
       </c>
       <c r="E29" t="s">
         <v>34</v>
@@ -2524,17 +2518,17 @@
       <c r="F29" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>35</v>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" t="s">
+        <v>34</v>
       </c>
       <c r="K29" t="s">
         <v>34</v>
@@ -2557,512 +2551,510 @@
       <c r="Q29" t="s">
         <v>34</v>
       </c>
-      <c r="R29" s="5" t="s">
-        <v>35</v>
+      <c r="R29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="43"/>
+      <c r="B30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30" t="s">
+        <v>34</v>
+      </c>
+      <c r="N30" t="s">
+        <v>34</v>
+      </c>
+      <c r="O30" t="s">
+        <v>34</v>
+      </c>
+      <c r="P30" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>34</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="43"/>
+      <c r="B31" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31" t="s">
+        <v>34</v>
+      </c>
+      <c r="O31" t="s">
+        <v>34</v>
+      </c>
+      <c r="P31" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>34</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="43"/>
+      <c r="B32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32" t="s">
+        <v>34</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P32" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>34</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J33" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" t="s">
+        <v>34</v>
+      </c>
+      <c r="L33" t="s">
+        <v>34</v>
+      </c>
+      <c r="M33" t="s">
+        <v>34</v>
+      </c>
+      <c r="N33" t="s">
+        <v>34</v>
+      </c>
+      <c r="O33" t="s">
+        <v>34</v>
+      </c>
+      <c r="P33" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>34</v>
+      </c>
+      <c r="R33" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="44"/>
+      <c r="B34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I34" t="s">
+        <v>34</v>
+      </c>
+      <c r="J34" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" t="s">
+        <v>34</v>
+      </c>
+      <c r="L34" t="s">
+        <v>34</v>
+      </c>
+      <c r="M34" t="s">
+        <v>34</v>
+      </c>
+      <c r="N34" t="s">
+        <v>34</v>
+      </c>
+      <c r="O34" t="s">
+        <v>34</v>
+      </c>
+      <c r="P34" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>34</v>
+      </c>
+      <c r="R34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K35" t="s">
+        <v>34</v>
+      </c>
+      <c r="L35" t="s">
+        <v>34</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N35" t="s">
+        <v>34</v>
+      </c>
+      <c r="O35" t="s">
+        <v>34</v>
+      </c>
+      <c r="P35" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>34</v>
+      </c>
+      <c r="R35" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" t="s">
-        <v>34</v>
-      </c>
-      <c r="I30" t="s">
-        <v>34</v>
-      </c>
-      <c r="J30" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" t="s">
-        <v>34</v>
-      </c>
-      <c r="L30" t="s">
-        <v>34</v>
-      </c>
-      <c r="M30" t="s">
-        <v>34</v>
-      </c>
-      <c r="N30" t="s">
-        <v>34</v>
-      </c>
-      <c r="O30" t="s">
-        <v>34</v>
-      </c>
-      <c r="P30" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>34</v>
-      </c>
-      <c r="R30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="25"/>
-      <c r="B31" s="10" t="s">
+      <c r="C36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K36" t="s">
+        <v>34</v>
+      </c>
+      <c r="L36" t="s">
+        <v>34</v>
+      </c>
+      <c r="M36" t="s">
+        <v>34</v>
+      </c>
+      <c r="N36" t="s">
+        <v>34</v>
+      </c>
+      <c r="O36" t="s">
+        <v>34</v>
+      </c>
+      <c r="P36" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>34</v>
+      </c>
+      <c r="R36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="43"/>
+      <c r="B37" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C31" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" t="s">
-        <v>34</v>
-      </c>
-      <c r="M31" t="s">
-        <v>34</v>
-      </c>
-      <c r="N31" t="s">
-        <v>34</v>
-      </c>
-      <c r="O31" t="s">
-        <v>34</v>
-      </c>
-      <c r="P31" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>34</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="25"/>
-      <c r="B32" s="10" t="s">
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37" t="s">
+        <v>34</v>
+      </c>
+      <c r="I37" t="s">
+        <v>34</v>
+      </c>
+      <c r="J37" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" t="s">
+        <v>34</v>
+      </c>
+      <c r="L37" t="s">
+        <v>34</v>
+      </c>
+      <c r="M37" t="s">
+        <v>34</v>
+      </c>
+      <c r="N37" t="s">
+        <v>34</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P37" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>34</v>
+      </c>
+      <c r="R37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="43"/>
+      <c r="B38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G32" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" t="s">
-        <v>34</v>
-      </c>
-      <c r="J32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32" t="s">
-        <v>34</v>
-      </c>
-      <c r="L32" t="s">
-        <v>34</v>
-      </c>
-      <c r="M32" t="s">
-        <v>34</v>
-      </c>
-      <c r="N32" t="s">
-        <v>34</v>
-      </c>
-      <c r="O32" t="s">
-        <v>34</v>
-      </c>
-      <c r="P32" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>34</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18">
-      <c r="A33" s="25"/>
-      <c r="B33" s="10" t="s">
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K38" t="s">
+        <v>34</v>
+      </c>
+      <c r="L38" t="s">
+        <v>34</v>
+      </c>
+      <c r="M38" t="s">
+        <v>34</v>
+      </c>
+      <c r="N38" t="s">
+        <v>34</v>
+      </c>
+      <c r="O38" t="s">
+        <v>34</v>
+      </c>
+      <c r="P38" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>34</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="43"/>
+      <c r="B39" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K33" t="s">
-        <v>34</v>
-      </c>
-      <c r="L33" t="s">
-        <v>34</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N33" t="s">
-        <v>34</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P33" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>34</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18">
-      <c r="A34" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" t="s">
-        <v>34</v>
-      </c>
-      <c r="H34" t="s">
-        <v>34</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J34" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" t="s">
-        <v>34</v>
-      </c>
-      <c r="L34" t="s">
-        <v>34</v>
-      </c>
-      <c r="M34" t="s">
-        <v>34</v>
-      </c>
-      <c r="N34" t="s">
-        <v>34</v>
-      </c>
-      <c r="O34" t="s">
-        <v>34</v>
-      </c>
-      <c r="P34" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>34</v>
-      </c>
-      <c r="R34" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18">
-      <c r="A35" s="26"/>
-      <c r="B35" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" t="s">
-        <v>34</v>
-      </c>
-      <c r="H35" t="s">
-        <v>34</v>
-      </c>
-      <c r="I35" t="s">
-        <v>34</v>
-      </c>
-      <c r="J35" t="s">
-        <v>34</v>
-      </c>
-      <c r="K35" t="s">
-        <v>34</v>
-      </c>
-      <c r="L35" t="s">
-        <v>34</v>
-      </c>
-      <c r="M35" t="s">
-        <v>34</v>
-      </c>
-      <c r="N35" t="s">
-        <v>34</v>
-      </c>
-      <c r="O35" t="s">
-        <v>34</v>
-      </c>
-      <c r="P35" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>34</v>
-      </c>
-      <c r="R35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18">
-      <c r="A36" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K36" t="s">
-        <v>34</v>
-      </c>
-      <c r="L36" t="s">
-        <v>34</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N36" t="s">
-        <v>34</v>
-      </c>
-      <c r="O36" t="s">
-        <v>34</v>
-      </c>
-      <c r="P36" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>34</v>
-      </c>
-      <c r="R36" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18">
-      <c r="A37" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" t="s">
-        <v>34</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K37" t="s">
-        <v>34</v>
-      </c>
-      <c r="L37" t="s">
-        <v>34</v>
-      </c>
-      <c r="M37" t="s">
-        <v>34</v>
-      </c>
-      <c r="N37" t="s">
-        <v>34</v>
-      </c>
-      <c r="O37" t="s">
-        <v>34</v>
-      </c>
-      <c r="P37" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>34</v>
-      </c>
-      <c r="R37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18">
-      <c r="A38" s="25"/>
-      <c r="B38" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" t="s">
-        <v>34</v>
-      </c>
-      <c r="G38" t="s">
-        <v>34</v>
-      </c>
-      <c r="H38" t="s">
-        <v>34</v>
-      </c>
-      <c r="I38" t="s">
-        <v>34</v>
-      </c>
-      <c r="J38" t="s">
-        <v>34</v>
-      </c>
-      <c r="K38" t="s">
-        <v>34</v>
-      </c>
-      <c r="L38" t="s">
-        <v>34</v>
-      </c>
-      <c r="M38" t="s">
-        <v>34</v>
-      </c>
-      <c r="N38" t="s">
-        <v>34</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P38" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>34</v>
-      </c>
-      <c r="R38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18">
-      <c r="A39" s="25"/>
-      <c r="B39" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" t="s">
-        <v>34</v>
+      <c r="C39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E39" t="s">
         <v>34</v>
@@ -3082,20 +3074,20 @@
       <c r="J39" t="s">
         <v>34</v>
       </c>
-      <c r="K39" t="s">
-        <v>34</v>
+      <c r="K39" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="L39" t="s">
         <v>34</v>
       </c>
-      <c r="M39" t="s">
-        <v>34</v>
-      </c>
-      <c r="N39" t="s">
-        <v>34</v>
-      </c>
-      <c r="O39" t="s">
-        <v>34</v>
+      <c r="M39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="P39" t="s">
         <v>34</v>
@@ -3103,19 +3095,19 @@
       <c r="Q39" t="s">
         <v>34</v>
       </c>
-      <c r="R39" s="1" t="s">
-        <v>35</v>
+      <c r="R39" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="25"/>
-      <c r="B40" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="A40" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="28"/>
+      <c r="C40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E40" t="s">
@@ -3130,362 +3122,336 @@
       <c r="H40" t="s">
         <v>34</v>
       </c>
-      <c r="I40" t="s">
-        <v>34</v>
+      <c r="I40" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="J40" t="s">
         <v>34</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L40" t="s">
-        <v>34</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>35</v>
+      <c r="K40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M40" t="s">
+        <v>34</v>
+      </c>
+      <c r="N40" t="s">
+        <v>34</v>
+      </c>
+      <c r="O40" t="s">
+        <v>34</v>
       </c>
       <c r="P40" t="s">
         <v>34</v>
       </c>
-      <c r="Q40" t="s">
-        <v>34</v>
-      </c>
-      <c r="R40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
-      <c r="A41" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="24"/>
-      <c r="C41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E41" t="s">
-        <v>34</v>
-      </c>
-      <c r="F41" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" t="s">
-        <v>34</v>
-      </c>
-      <c r="H41" t="s">
-        <v>34</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J41" t="s">
-        <v>34</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M41" t="s">
-        <v>34</v>
-      </c>
-      <c r="N41" t="s">
-        <v>34</v>
-      </c>
-      <c r="O41" t="s">
-        <v>34</v>
-      </c>
-      <c r="P41" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q41" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R41" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" s="3" customFormat="1" ht="140.25">
-      <c r="A42" s="31" t="s">
+      <c r="Q40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R40" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" s="3" customFormat="1" ht="140.25">
+      <c r="A41" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="7" t="s">
+      <c r="B41" s="42"/>
+      <c r="C41" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E41" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H42" s="7" t="s">
+      <c r="H41" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I41" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J42" s="7" t="s">
+      <c r="J41" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K42" s="6" t="s">
+      <c r="K41" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L42" s="7" t="s">
+      <c r="L41" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="M42" s="7" t="s">
+      <c r="M41" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="N42" s="7" t="s">
+      <c r="N41" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="O42" s="7" t="s">
+      <c r="O41" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="P42" s="7" t="s">
+      <c r="P41" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="Q42" s="7" t="s">
+      <c r="Q41" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="R42" s="7" t="s">
+      <c r="R41" s="7" t="s">
         <v>93</v>
       </c>
     </row>
+    <row r="42" spans="1:18">
+      <c r="A42" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" t="s">
+        <v>34</v>
+      </c>
+      <c r="J42" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42" t="s">
+        <v>34</v>
+      </c>
+      <c r="L42" t="s">
+        <v>34</v>
+      </c>
+      <c r="M42" t="s">
+        <v>34</v>
+      </c>
+      <c r="N42" t="s">
+        <v>34</v>
+      </c>
+      <c r="O42" t="s">
+        <v>34</v>
+      </c>
+      <c r="P42" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>34</v>
+      </c>
+      <c r="R42" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="24"/>
+      <c r="A43" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="28"/>
       <c r="C43" t="s">
         <v>34</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>35</v>
+      <c r="E43" t="s">
+        <v>34</v>
       </c>
       <c r="F43" t="s">
         <v>34</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>35</v>
+      <c r="G43" t="s">
+        <v>34</v>
       </c>
       <c r="H43" t="s">
         <v>34</v>
       </c>
-      <c r="I43" t="s">
-        <v>34</v>
-      </c>
-      <c r="J43" t="s">
-        <v>34</v>
-      </c>
-      <c r="K43" t="s">
-        <v>34</v>
+      <c r="I43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="L43" t="s">
         <v>34</v>
       </c>
-      <c r="M43" t="s">
-        <v>34</v>
+      <c r="M43" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="N43" t="s">
         <v>34</v>
       </c>
-      <c r="O43" t="s">
-        <v>34</v>
-      </c>
-      <c r="P43" t="s">
-        <v>34</v>
+      <c r="O43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P43" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="Q43" t="s">
         <v>34</v>
       </c>
-      <c r="R43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18">
-      <c r="A44" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G44" t="s">
-        <v>34</v>
-      </c>
-      <c r="H44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L44" t="s">
-        <v>34</v>
-      </c>
-      <c r="M44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N44" t="s">
-        <v>34</v>
-      </c>
-      <c r="O44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P44" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>34</v>
-      </c>
-      <c r="R44" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" s="3" customFormat="1" ht="92.25" customHeight="1">
+      <c r="R43" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" s="3" customFormat="1" ht="92.25" customHeight="1">
+      <c r="A44" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="D44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q44" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R44" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" s="3" customFormat="1" ht="75" customHeight="1">
       <c r="A45" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="36"/>
-      <c r="D45" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="N45" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="O45" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="P45" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q45" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="R45" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" s="3" customFormat="1" ht="75" customHeight="1">
-      <c r="A46" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" s="34"/>
-      <c r="D46" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="19" t="s">
+      <c r="G45" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H45" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="J46" s="17"/>
-      <c r="M46" s="4" t="s">
+      <c r="J45" s="17"/>
+      <c r="M45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N46" s="19" t="s">
+      <c r="N45" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="O46" s="4" t="s">
+      <c r="O45" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P46" s="4" t="s">
+      <c r="P45" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Q46" s="19" t="s">
+      <c r="Q45" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="R46" s="4" t="s">
+      <c r="R45" s="4" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="16" t="s">
         <v>98</v>
       </c>
     </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="13" t="s">
-        <v>87</v>
+      <c r="A53" s="14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="14" t="s">
-        <v>43</v>
+      <c r="A54" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="20" t="s">
+      <c r="A55" s="19" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="39">
+  <mergeCells count="38">
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
@@ -3496,35 +3462,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed incorrect analysis of template parameters (Scala bug?)
</commit_message>
<xml_diff>
--- a/xslt-collection/features.xlsx
+++ b/xslt-collection/features.xlsx
@@ -548,43 +548,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -599,11 +573,37 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -964,7 +964,7 @@
   <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -990,8 +990,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="8" customFormat="1">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
+      <c r="A1" s="35"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1042,10 +1042,10 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="40"/>
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1096,10 +1096,10 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="42"/>
       <c r="C3" t="s">
         <v>26</v>
       </c>
@@ -1150,10 +1150,10 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="44"/>
       <c r="C4" t="s">
         <v>34</v>
       </c>
@@ -1204,10 +1204,10 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="34"/>
       <c r="C5" t="s">
         <v>34</v>
       </c>
@@ -1258,10 +1258,10 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="38"/>
       <c r="C6" t="s">
         <v>34</v>
       </c>
@@ -1312,10 +1312,10 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="38"/>
       <c r="C7" t="s">
         <v>34</v>
       </c>
@@ -1366,10 +1366,10 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="40"/>
+      <c r="B8" s="26"/>
       <c r="C8" t="s">
         <v>34</v>
       </c>
@@ -1420,10 +1420,10 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="34"/>
       <c r="C9" t="s">
         <v>34</v>
       </c>
@@ -1474,10 +1474,10 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1528,12 +1528,12 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
+      <c r="B11" s="22"/>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>35</v>
@@ -1541,32 +1541,32 @@
       <c r="E11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>35</v>
+      <c r="F11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>35</v>
+      <c r="H11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>35</v>
+      <c r="J11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="K11" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>35</v>
+      <c r="L11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="5" t="s">
-        <v>35</v>
+      <c r="N11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>35</v>
@@ -1577,15 +1577,15 @@
       <c r="Q11" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="5" t="s">
-        <v>35</v>
+      <c r="R11" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="22"/>
       <c r="C12" t="s">
         <v>34</v>
       </c>
@@ -1636,10 +1636,10 @@
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="22"/>
       <c r="C13" t="s">
         <v>34</v>
       </c>
@@ -1690,10 +1690,10 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="40"/>
+      <c r="B14" s="26"/>
       <c r="C14" t="s">
         <v>34</v>
       </c>
@@ -1744,10 +1744,10 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="5" t="s">
         <v>35</v>
       </c>
@@ -1798,10 +1798,10 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="22"/>
       <c r="C16" t="s">
         <v>34</v>
       </c>
@@ -1852,10 +1852,10 @@
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="22"/>
       <c r="C17" t="s">
         <v>34</v>
       </c>
@@ -1906,10 +1906,10 @@
       </c>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="22"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -1960,10 +1960,10 @@
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="28"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="5" t="s">
         <v>35</v>
       </c>
@@ -2014,10 +2014,10 @@
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="28"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
@@ -2068,10 +2068,10 @@
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="28"/>
+      <c r="B21" s="22"/>
       <c r="C21" t="s">
         <v>34</v>
       </c>
@@ -2122,10 +2122,10 @@
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="26"/>
+      <c r="B22" s="34"/>
       <c r="C22" t="s">
         <v>34</v>
       </c>
@@ -2176,10 +2176,10 @@
       </c>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="40"/>
+      <c r="B23" s="26"/>
       <c r="C23" t="s">
         <v>34</v>
       </c>
@@ -2230,10 +2230,10 @@
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="28"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="5" t="s">
         <v>35</v>
       </c>
@@ -2284,10 +2284,10 @@
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="28"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="5" t="s">
         <v>35</v>
       </c>
@@ -2338,10 +2338,10 @@
       </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="26"/>
+      <c r="B26" s="34"/>
       <c r="C26" t="s">
         <v>34</v>
       </c>
@@ -2392,10 +2392,10 @@
       </c>
     </row>
     <row r="27" spans="1:18" s="3" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="42"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="7" t="s">
         <v>37</v>
       </c>
@@ -2446,10 +2446,10 @@
       </c>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="28"/>
+      <c r="B28" s="22"/>
       <c r="C28" s="5" t="s">
         <v>35</v>
       </c>
@@ -2500,7 +2500,7 @@
       </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -2556,7 +2556,7 @@
       </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="43"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="10" t="s">
         <v>33</v>
       </c>
@@ -2610,7 +2610,7 @@
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="43"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="10" t="s">
         <v>32</v>
       </c>
@@ -2664,7 +2664,7 @@
       </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="43"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="10" t="s">
         <v>31</v>
       </c>
@@ -2718,7 +2718,7 @@
       </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="24" t="s">
         <v>76</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -2774,7 +2774,7 @@
       </c>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="44"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="9" t="s">
         <v>45</v>
       </c>
@@ -2828,10 +2828,10 @@
       </c>
     </row>
     <row r="35" spans="1:18">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="28"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="5" t="s">
         <v>35</v>
       </c>
@@ -2882,7 +2882,7 @@
       </c>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="23" t="s">
         <v>78</v>
       </c>
       <c r="B36" s="10" t="s">
@@ -2938,7 +2938,7 @@
       </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="43"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="10" t="s">
         <v>33</v>
       </c>
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="43"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="10" t="s">
         <v>32</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="43"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="10" t="s">
         <v>31</v>
       </c>
@@ -3100,10 +3100,10 @@
       </c>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="28"/>
+      <c r="B40" s="22"/>
       <c r="C40" t="s">
         <v>34</v>
       </c>
@@ -3154,10 +3154,10 @@
       </c>
     </row>
     <row r="41" spans="1:18" s="3" customFormat="1" ht="140.25">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="42"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="7" t="s">
         <v>46</v>
       </c>
@@ -3208,10 +3208,10 @@
       </c>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="28"/>
+      <c r="B42" s="22"/>
       <c r="C42" t="s">
         <v>34</v>
       </c>
@@ -3262,10 +3262,10 @@
       </c>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="28"/>
+      <c r="B43" s="22"/>
       <c r="C43" t="s">
         <v>34</v>
       </c>
@@ -3316,10 +3316,10 @@
       </c>
     </row>
     <row r="44" spans="1:18" s="3" customFormat="1" ht="92.25" customHeight="1">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="38"/>
+      <c r="B44" s="32"/>
       <c r="D44" s="7" t="s">
         <v>47</v>
       </c>
@@ -3355,10 +3355,10 @@
       </c>
     </row>
     <row r="45" spans="1:18" s="3" customFormat="1" ht="75" customHeight="1">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="30"/>
       <c r="D45" s="4" t="s">
         <v>49</v>
       </c>
@@ -3424,18 +3424,16 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="38">
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A44:B44"/>
@@ -3452,16 +3450,18 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>